<commit_message>
Pembelajaran dan halaman errors
</commit_message>
<xml_diff>
--- a/public/format_excel/format_import_mapel.xlsx
+++ b/public/format_excel/format_import_mapel.xlsx
@@ -454,8 +454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10:C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -961,7 +961,7 @@
   </mergeCells>
   <dataValidations count="4">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Tahun Ajaran" prompt="Isikan tahun pelajaran sekarang. contoh &quot;2022/2023&quot; tanpa tanda kutip" sqref="B10:B59"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Kategori" prompt="Isikan data kategori mapel dengan kode berikut _x000a_1 = K-1_x000a_2 = K-2_x000a_3 = K-3_x000a_4 = K-4_x000a_5 = KO &amp; EKSTAKULIKULER_x000a_6 = MULOK KHAS PI_x000a_7 = PELAJARAN SHOLAT_x000a_8 = HAFALAN_x000a_9 = TAHSIN_x000a_10 = THAFIDZ_x000a_11 = BUDAYA PRIMA_x000a_12 = AMAL IBADAH" sqref="C10:C59"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Kategori" prompt="Isikan data kategori mapel dengan kode berikut _x000a_1 = K-1_x000a_2 = K-2_x000a_3 = K-3 dan K-4_x000a_5 = KO &amp; EKSTAKULIKULER_x000a_6 = MULOK KHAS PI_x000a_7 = PELAJARAN SHOLAT_x000a_8 = HAFALAN_x000a_9 = TAHSIN_x000a_10 = THAFIDZ_x000a_11 = BUDAYA PRIMA_x000a_12 = AMAL IBADAH" sqref="C10:C59"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Mata Pelajaran" prompt="Isikan dengan nama mata pelajaran" sqref="D10:D59"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Penjelasan Mapel" prompt="Isikan secara singkat keterangan mapel jika ada" sqref="E10:E59"/>
   </dataValidations>

</xml_diff>